<commit_message>
Mejorar el proceso de creación de empleados: actualizar los métodos para incluir la generación de un ID de empleado único y el guardado del formulario; agregar funcionalidad para marcar las filas de Excel como utilizadas.
</commit_message>
<xml_diff>
--- a/automatizacion/src/test/resources/datos.xlsx
+++ b/automatizacion/src/test/resources/datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yulia\proyecto-automatizacion\hocol-test\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.ladino\Automatizacion\ProjectMaven\automatizacion\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7230E0DC-E871-4F31-81E0-6440AFADBBB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84BF2E4-AAAF-460B-B272-BF43FB31D92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
+    <workbookView xWindow="20370" yWindow="-1815" windowWidth="29040" windowHeight="15720" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Estado</t>
   </si>
@@ -102,53 +102,41 @@
     <t>Fecha expiracion Licencia</t>
   </si>
   <si>
-    <t>2001-22-01</t>
-  </si>
-  <si>
-    <t>2001-22-02</t>
-  </si>
-  <si>
-    <t>2001-22-03</t>
-  </si>
-  <si>
-    <t>2001-22-04</t>
-  </si>
-  <si>
-    <t>2001-22-05</t>
-  </si>
-  <si>
-    <t>2001-22-06</t>
-  </si>
-  <si>
     <t>Fecha de Nacimiento</t>
   </si>
   <si>
-    <t>2019-22-01</t>
-  </si>
-  <si>
-    <t>2019-22-02</t>
-  </si>
-  <si>
-    <t>2019-22-03</t>
-  </si>
-  <si>
-    <t>2019-22-04</t>
-  </si>
-  <si>
-    <t>2019-22-05</t>
-  </si>
-  <si>
-    <t>2019-22-06</t>
-  </si>
-  <si>
     <t>Disponible</t>
+  </si>
+  <si>
+    <t>2019-01-22</t>
+  </si>
+  <si>
+    <t>2019-02-22</t>
+  </si>
+  <si>
+    <t>2019-03-22</t>
+  </si>
+  <si>
+    <t>2019-04-22</t>
+  </si>
+  <si>
+    <t>2019-05-22</t>
+  </si>
+  <si>
+    <t>2019-06-22</t>
+  </si>
+  <si>
+    <t>2001-01-22</t>
+  </si>
+  <si>
+    <t>2001-02-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,20 +511,20 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="21.75" customWidth="1"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="21.625" customWidth="1"/>
-    <col min="6" max="7" width="25.25" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="7" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -556,13 +544,13 @@
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -579,16 +567,16 @@
         <v>555551</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -605,16 +593,16 @@
         <v>555552</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -631,16 +619,16 @@
         <v>555553</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -657,16 +645,16 @@
         <v>555554</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -683,16 +671,16 @@
         <v>555555</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -709,13 +697,13 @@
         <v>555556</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactorizar el manejo del formulario de empleados: actualizar la duración de las pausas para una mejor observación, mejorar la lógica de selección de género e implementar el marcado de los registros de Excel como utilizados.
</commit_message>
<xml_diff>
--- a/automatizacion/src/test/resources/datos.xlsx
+++ b/automatizacion/src/test/resources/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.ladino\Automatizacion\ProjectMaven\automatizacion\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84BF2E4-AAAF-460B-B272-BF43FB31D92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DE269C-EB88-465A-A391-0941E3DA67F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1815" windowWidth="29040" windowHeight="15720" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Estado</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>2001-02-22</t>
+  </si>
+  <si>
+    <t>Usado</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>Hombre</t>
   </si>
 </sst>
 </file>
@@ -508,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EA86F-2CF4-4D61-97BB-1D094DEA001F}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +533,10 @@
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="7" width="25.28515625" customWidth="1"/>
+    <col min="6" max="8" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -547,10 +559,13 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -572,63 +587,72 @@
       <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>105369875</v>
+        <v>105369876</v>
       </c>
       <c r="E3">
-        <v>555552</v>
+        <v>555553</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>105369876</v>
+        <v>105369875</v>
       </c>
       <c r="E4">
-        <v>555553</v>
+        <v>555552</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -650,11 +674,14 @@
       <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -676,11 +703,14 @@
       <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -702,7 +732,10 @@
       <c r="G7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregar funcionalidad para capturar y adjuntar capturas de pantalla en los pasos de prueba; actualizar el proceso de creación de empleados para incluir el manejo de estado civil y nacionalidad; añadir archivos de configuración para los reportes de Extent.
</commit_message>
<xml_diff>
--- a/automatizacion/src/test/resources/datos.xlsx
+++ b/automatizacion/src/test/resources/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.ladino\Automatizacion\ProjectMaven\automatizacion\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DE269C-EB88-465A-A391-0941E3DA67F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CED3E41-24AB-46EA-9209-8B3BF8CD4D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1815" windowWidth="29040" windowHeight="15720" xr2:uid="{1B2942B2-1002-49AC-B066-AD15A2B34D50}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Estado</t>
   </si>
@@ -142,6 +142,39 @@
   </si>
   <si>
     <t>Hombre</t>
+  </si>
+  <si>
+    <t>Nacionalidad</t>
+  </si>
+  <si>
+    <t>Colombian</t>
+  </si>
+  <si>
+    <t>Angolan</t>
+  </si>
+  <si>
+    <t>Bolivian</t>
+  </si>
+  <si>
+    <t>Peruvian</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>Estado Civil</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -520,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EA86F-2CF4-4D61-97BB-1D094DEA001F}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +566,10 @@
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="6" max="8" width="25.28515625" customWidth="1"/>
+    <col min="6" max="10" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -559,13 +592,19 @@
         <v>25</v>
       </c>
       <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -588,13 +627,19 @@
         <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -617,13 +662,19 @@
         <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I3" t="s">
-        <v>26</v>
+      <c r="K3" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -646,13 +697,19 @@
         <v>34</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -675,13 +732,19 @@
         <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -704,13 +767,19 @@
         <v>34</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -733,9 +802,15 @@
         <v>34</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>